<commit_message>
Atualização Mapeamento Conferência - NIKE e BUNZL
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_BUNZL.xlsx
+++ b/Documentação/Planilhas/Conferencia_BUNZL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7725" tabRatio="745" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7725" tabRatio="745" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="VW_BZL_Clientes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="293">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -893,6 +893,12 @@
   </si>
   <si>
     <t>Fazer o detalhamento da linha apresentada. Na aba inferior "Pedido de Vendas Site - Linhas", pegar a informação da Data de Aprovação. Caso esse campo não esteja visivel, configurar a tela para apresentá-lo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTSX: </t>
+  </si>
+  <si>
+    <t>N:\Migracao\Bunzl_Carga\Bunzl\Bunzl.sln</t>
   </si>
 </sst>
 </file>
@@ -1290,6 +1296,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1301,9 +1317,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1349,6 +1362,36 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1357,43 +1400,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1698,10 +1704,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:R31"/>
+  <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1742,222 +1748,174 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="4" spans="1:18" ht="23.25" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="23.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:18" s="8" customFormat="1">
+      <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q8" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="R7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="8" customFormat="1">
-      <c r="A8" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="8" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>150</v>
@@ -1966,363 +1924,419 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A11" s="22" t="s">
+    <row r="10" spans="1:18" s="8" customFormat="1">
+      <c r="A10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" ht="11.25" customHeight="1">
+      <c r="A12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="27"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="32"/>
     </row>
     <row r="13" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="35"/>
     </row>
     <row r="14" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="35"/>
     </row>
     <row r="15" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="38"/>
+    </row>
+    <row r="16" spans="1:18" ht="11.25" customHeight="1">
+      <c r="A16" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C16" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D16" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E16" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F16" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G16" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H16" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I16" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J16" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K16" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L16" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M16" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N16" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="O15" s="31" t="s">
+      <c r="O16" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="P15" s="31" t="s">
+      <c r="P16" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="Q15" s="31" t="s">
+      <c r="Q16" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="R15" s="31" t="s">
+      <c r="R16" s="29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-    </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-    </row>
-    <row r="24" spans="1:18" ht="11.25" customHeight="1">
-      <c r="Q24" s="31" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+    </row>
+    <row r="25" spans="1:18" ht="11.25" customHeight="1">
+      <c r="Q25" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="R24" s="31" t="s">
+      <c r="R25" s="29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
-    </row>
     <row r="26" spans="1:18">
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
     </row>
     <row r="28" spans="1:18">
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="Q31" s="31"/>
-      <c r="R31" s="31"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="P15:P22"/>
-    <mergeCell ref="E15:E22"/>
-    <mergeCell ref="J15:J22"/>
-    <mergeCell ref="L15:L22"/>
-    <mergeCell ref="M15:M22"/>
-    <mergeCell ref="A11:R14"/>
-    <mergeCell ref="Q24:Q31"/>
-    <mergeCell ref="R24:R31"/>
-    <mergeCell ref="F15:F22"/>
-    <mergeCell ref="Q15:Q22"/>
-    <mergeCell ref="R15:R22"/>
-    <mergeCell ref="C15:C22"/>
-    <mergeCell ref="K15:K22"/>
-    <mergeCell ref="G15:G22"/>
-    <mergeCell ref="H15:H22"/>
-    <mergeCell ref="I15:I22"/>
-    <mergeCell ref="O15:O22"/>
-    <mergeCell ref="N15:N22"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="D15:D22"/>
+    <mergeCell ref="A12:R15"/>
+    <mergeCell ref="Q25:Q32"/>
+    <mergeCell ref="R25:R32"/>
+    <mergeCell ref="F16:F23"/>
+    <mergeCell ref="Q16:Q23"/>
+    <mergeCell ref="R16:R23"/>
+    <mergeCell ref="C16:C23"/>
+    <mergeCell ref="K16:K23"/>
+    <mergeCell ref="G16:G23"/>
+    <mergeCell ref="H16:H23"/>
+    <mergeCell ref="I16:I23"/>
+    <mergeCell ref="O16:O23"/>
+    <mergeCell ref="N16:N23"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="D16:D23"/>
+    <mergeCell ref="P16:P23"/>
+    <mergeCell ref="E16:E23"/>
+    <mergeCell ref="J16:J23"/>
+    <mergeCell ref="L16:L23"/>
+    <mergeCell ref="M16:M23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2334,10 +2348,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:K36"/>
+  <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2372,81 +2386,54 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="4" spans="1:11" ht="23.25" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="23.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2458,58 +2445,58 @@
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>118</v>
+      <c r="H9" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
@@ -2528,49 +2515,49 @@
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>22</v>
+      <c r="H10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>140</v>
+        <v>112</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>144</v>
+      <c r="H11" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>22</v>
@@ -2582,30 +2569,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="8" customFormat="1">
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>118</v>
+      <c r="H12" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -2621,26 +2608,26 @@
       <c r="A13" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="B13" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>35</v>
+      <c r="H13" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>22</v>
@@ -2653,296 +2640,331 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="8" customFormat="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="22" t="s">
+      <c r="A14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="11.25" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34"/>
-    </row>
-    <row r="17" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="37"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="11.25" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="44"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="44"/>
     </row>
     <row r="20" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+    </row>
+    <row r="21" spans="1:11" ht="11.25" customHeight="1">
+      <c r="A21" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B21" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C21" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D21" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E21" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F21" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G21" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I21" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="J21" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K20" s="31" t="s">
+      <c r="K21" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-    </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="31" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B30" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F30" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G30" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H30" s="39" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-    </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I20:I27"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="F29:F36"/>
-    <mergeCell ref="G29:G36"/>
-    <mergeCell ref="H29:H36"/>
-    <mergeCell ref="C16:K19"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="K20:K27"/>
-    <mergeCell ref="J20:J27"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="E20:E27"/>
-    <mergeCell ref="F20:F27"/>
-    <mergeCell ref="G20:G27"/>
-    <mergeCell ref="H20:H27"/>
-    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="C17:K20"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="K21:K28"/>
+    <mergeCell ref="J21:J28"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="D21:D28"/>
+    <mergeCell ref="E21:E28"/>
+    <mergeCell ref="F21:F28"/>
+    <mergeCell ref="G21:G28"/>
+    <mergeCell ref="H21:H28"/>
+    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="I21:I28"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="F30:F37"/>
+    <mergeCell ref="G30:G37"/>
+    <mergeCell ref="H30:H37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2954,10 +2976,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:O25"/>
+  <dimension ref="A2:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2996,142 +3018,103 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="23.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="4" spans="1:15" ht="23.25" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="23.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>7</v>
@@ -3139,10 +3122,10 @@
     </row>
     <row r="9" spans="1:15" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>14</v>
@@ -3175,7 +3158,7 @@
         <v>194</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>189</v>
+        <v>39</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>8</v>
@@ -3185,303 +3168,350 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-    </row>
-    <row r="11" spans="1:15" s="8" customFormat="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="22" t="s">
+      <c r="A10" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" s="8" customFormat="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" ht="11.25" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="34"/>
-    </row>
-    <row r="14" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="11.25" customHeight="1">
       <c r="A15" s="20"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="37"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="40"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="47"/>
+    </row>
+    <row r="18" spans="1:15" ht="11.25" customHeight="1">
+      <c r="A18" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B18" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C18" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D18" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E18" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F18" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G18" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H18" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="I17" s="31" t="s">
+      <c r="I18" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J18" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K18" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="L17" s="31" t="s">
+      <c r="L18" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="M17" s="31" t="s">
+      <c r="M18" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="N17" s="31" t="s">
+      <c r="N18" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="O17" s="31" t="s">
+      <c r="O18" s="29" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-    </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-    </row>
-    <row r="25" spans="1:15" ht="12" customHeight="1"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+    </row>
+    <row r="26" spans="1:15" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A17:A24"/>
-    <mergeCell ref="L17:L24"/>
-    <mergeCell ref="D17:D24"/>
-    <mergeCell ref="B17:B24"/>
-    <mergeCell ref="C17:C24"/>
-    <mergeCell ref="F17:F24"/>
-    <mergeCell ref="G17:G24"/>
-    <mergeCell ref="H17:H24"/>
-    <mergeCell ref="I17:I24"/>
-    <mergeCell ref="J17:J24"/>
-    <mergeCell ref="K17:K24"/>
-    <mergeCell ref="B13:O16"/>
-    <mergeCell ref="M17:M24"/>
-    <mergeCell ref="N17:N24"/>
-    <mergeCell ref="O17:O24"/>
-    <mergeCell ref="E17:E24"/>
+    <mergeCell ref="B14:O17"/>
+    <mergeCell ref="M18:M25"/>
+    <mergeCell ref="N18:N25"/>
+    <mergeCell ref="O18:O25"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="L18:L25"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="F18:F25"/>
+    <mergeCell ref="G18:G25"/>
+    <mergeCell ref="H18:H25"/>
+    <mergeCell ref="I18:I25"/>
+    <mergeCell ref="J18:J25"/>
+    <mergeCell ref="K18:K25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3493,10 +3523,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F17"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3526,44 +3556,32 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="4" spans="1:6" ht="23.25" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="23.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
@@ -3571,19 +3589,19 @@
         <v>205</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
@@ -3591,39 +3609,39 @@
         <v>205</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="A10" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>213</v>
+      <c r="E10" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
@@ -3631,156 +3649,176 @@
         <v>212</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A14" s="19"/>
-      <c r="B14" s="41" t="s">
+    <row r="13" spans="1:6" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="11.25" customHeight="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-    </row>
-    <row r="15" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:6" ht="11.25" customHeight="1">
       <c r="A16" s="20"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
     </row>
     <row r="18" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="1:6" ht="11.25" customHeight="1">
+      <c r="A19" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B19" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C19" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D19" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E19" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F19" s="29" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-    </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-    </row>
-    <row r="26" spans="1:6" ht="12" customHeight="1"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+    </row>
+    <row r="27" spans="1:6" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B14:F17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F18:F25"/>
+    <mergeCell ref="B15:F18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="F19:F26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3792,10 +3830,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:H44"/>
+  <dimension ref="A2:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3827,110 +3865,94 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="4" spans="1:8" ht="23.25" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="23.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B7" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="2" t="s">
+      <c r="C7" s="54"/>
+      <c r="D7" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>236</v>
-      </c>
-      <c r="C8" s="65"/>
+        <v>229</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="55"/>
       <c r="D8" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>230</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="55"/>
+      <c r="D9" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="C10" s="66"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="9" t="s">
         <v>283</v>
       </c>
@@ -3948,86 +3970,100 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" s="58" t="s">
+      <c r="A11" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="C11" s="56"/>
+      <c r="D11" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>244</v>
+      <c r="G11" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B12" s="58" t="s">
-        <v>247</v>
-      </c>
-      <c r="C12" s="58"/>
+        <v>242</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="57"/>
       <c r="D12" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>0</v>
+        <v>243</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" s="58"/>
+        <v>245</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="C13" s="57"/>
       <c r="D13" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>239</v>
+        <v>277</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="A14" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="11"/>
@@ -4049,260 +4085,274 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="41" t="s">
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="12" customHeight="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="11.25" customHeight="1">
+      <c r="A19" s="19"/>
+      <c r="B19" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="64"/>
     </row>
     <row r="20" spans="1:8" ht="11.25" customHeight="1">
       <c r="A20" s="20"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="48"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="65"/>
     </row>
     <row r="21" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="49"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="65"/>
     </row>
     <row r="22" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="66"/>
+    </row>
+    <row r="23" spans="1:8" ht="11.25" customHeight="1">
+      <c r="A23" s="29" t="s">
         <v>278</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B23" s="58" t="s">
         <v>279</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="31" t="s">
+      <c r="C23" s="59"/>
+      <c r="D23" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E23" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F23" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G23" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H23" s="29" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="31"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-    </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="31"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="31"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="31"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="31"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="31"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="31"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" ht="12" customHeight="1"/>
-    <row r="32" spans="1:8">
-      <c r="B32" s="50" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="29"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+    </row>
+    <row r="31" spans="1:8" ht="12" customHeight="1"/>
+    <row r="33" spans="2:3">
+      <c r="B33" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C33" s="22" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="51" t="s">
+    <row r="34" spans="2:3">
+      <c r="B34" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C34" s="24" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="53" t="s">
+    <row r="35" spans="2:3">
+      <c r="B35" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C35" s="26" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="53" t="s">
+    <row r="36" spans="2:3">
+      <c r="B36" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C36" s="26" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="53" t="s">
+    <row r="37" spans="2:3">
+      <c r="B37" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C37" s="26" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="53" t="s">
+    <row r="38" spans="2:3">
+      <c r="B38" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C38" s="26" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="53" t="s">
+    <row r="39" spans="2:3">
+      <c r="B39" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="C39" s="26" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="53" t="s">
+    <row r="40" spans="2:3">
+      <c r="B40" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="C39" s="54" t="s">
+      <c r="C40" s="26" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="53" t="s">
+    <row r="41" spans="2:3">
+      <c r="B41" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C40" s="54" t="s">
+      <c r="C41" s="26" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="53" t="s">
+    <row r="42" spans="2:3">
+      <c r="B42" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="C41" s="54" t="s">
+      <c r="C42" s="26" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="53" t="s">
+    <row r="43" spans="2:3">
+      <c r="B43" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C43" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="53" t="s">
+    <row r="44" spans="2:3">
+      <c r="B44" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C44" s="26" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="55" t="s">
+    <row r="45" spans="2:3">
+      <c r="B45" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C45" s="28" t="s">
         <v>254</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="E23:E30"/>
+    <mergeCell ref="F23:F30"/>
+    <mergeCell ref="G23:G30"/>
+    <mergeCell ref="H23:H30"/>
+    <mergeCell ref="D23:D30"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -4310,13 +4360,9 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B22:C29"/>
-    <mergeCell ref="B18:H21"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F22:F29"/>
-    <mergeCell ref="G22:G29"/>
-    <mergeCell ref="H22:H29"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B23:C30"/>
+    <mergeCell ref="B19:H22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>